<commit_message>
logical functions & math functions
</commit_message>
<xml_diff>
--- a/2_Formulas_Functions/3_Logical_Functions.xlsx
+++ b/2_Formulas_Functions/3_Logical_Functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Developer\_Courses\Excel\Excel_Data_Analytics_Course\2_Formulas_Functions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajay/Documents/Personal/Courses/Data Scientist/Learn_Excel/Excel_DA_Course/2_Formulas_Functions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DACF0C-E6D1-403B-A48D-03B483E33508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F437611-AD72-5B46-9A99-DA73002BFBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-102" yWindow="1488" windowWidth="18372" windowHeight="10296" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_1" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -866,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -950,7 +950,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -962,7 +961,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1321,36 +1320,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D423364-12D3-4C3A-8A6B-C3645EBFE927}">
   <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="11.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.26171875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.15625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.41796875" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.68359375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.15625" style="1"/>
-    <col min="18" max="18" width="14.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" style="1"/>
+    <col min="18" max="18" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25"/>
     </row>
-    <row r="2" spans="2:17" s="11" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:17" s="11" customFormat="1" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1400,7 +1399,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1457,9 +1456,12 @@
         <f>AND(L3,M3)</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="32"/>
-    </row>
-    <row r="4" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q3" s="32" t="str">
+        <f>IF(P3,"Goal Met", "Not Met")</f>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1516,9 +1518,12 @@
         <f t="shared" ref="P4:P12" si="10">AND(L4,M4)</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="32"/>
-    </row>
-    <row r="5" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q4" s="32" t="str">
+        <f t="shared" ref="Q4:Q12" si="11">IF(P4,"Goal Met", "Not Met")</f>
+        <v>Not Met</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1575,9 +1580,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q5" s="32"/>
-    </row>
-    <row r="6" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q5" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Not Met</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1634,9 +1642,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="32"/>
-    </row>
-    <row r="7" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q6" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1693,9 +1704,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="32"/>
-    </row>
-    <row r="8" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q7" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Not Met</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1752,9 +1766,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q8" s="32"/>
-    </row>
-    <row r="9" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q8" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1811,9 +1828,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="32"/>
-    </row>
-    <row r="10" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q9" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
@@ -1870,9 +1890,12 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="32"/>
-    </row>
-    <row r="11" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q10" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1929,9 +1952,12 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="32"/>
-    </row>
-    <row r="12" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q11" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Not Met</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -1988,14 +2014,17 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="Q12" s="33"/>
-    </row>
-    <row r="14" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="Q12" s="32" t="str">
+        <f t="shared" si="11"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>22</v>
       </c>
@@ -2003,7 +2032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>23</v>
       </c>
@@ -2013,6 +2042,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2024,33 +2054,33 @@
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.68359375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26171875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.578125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="11.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.26171875" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="9.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.41796875" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="14.15625" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="9.68359375" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.68359375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.15625" style="1"/>
-    <col min="19" max="19" width="14.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" style="1"/>
+    <col min="19" max="19" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G1" s="25"/>
     </row>
-    <row r="2" spans="2:17" s="11" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:17" s="11" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -2100,7 +2130,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -2162,7 +2192,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -2224,7 +2254,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -2286,7 +2316,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -2348,7 +2378,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="7" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -2410,7 +2440,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -2472,7 +2502,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -2534,7 +2564,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
@@ -2596,7 +2626,7 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="11" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
@@ -2658,7 +2688,7 @@
         <v>Not Met</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>9</v>
       </c>
@@ -2720,12 +2750,12 @@
         <v>Goal Met</v>
       </c>
     </row>
-    <row r="14" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>22</v>
       </c>
@@ -2733,7 +2763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>23</v>
       </c>
@@ -2750,33 +2780,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18E6D21-2229-4383-8B9A-431F68FAE08C}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.15625" customWidth="1"/>
-    <col min="3" max="3" width="21.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="68.15625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.9453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5234375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.3125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.41796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.05078125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="68.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="7.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>46</v>
       </c>
@@ -2832,11 +2861,11 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="46">
         <v>44996.547291666669</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -2863,12 +2892,44 @@
       <c r="J2" s="27" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" t="str">
+        <f>IF($A2=K$1, "Role Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="L2" t="str">
+        <f>IF($A2=L$1, "Role Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="M2" t="str">
+        <f>IF($A2=K$1, "Role Desired", IF($A2=L$1, "Role Desired", "Not Desired"))</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="N2" t="b">
+        <f>AND($A2=$K$1,$A2=$L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <f>OR($A2=$K$1, $A2=$L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="P2" t="str">
+        <f>IF(OR($A2=$K$1, $A2=$L$1), "Role Desired", "Not Desired")</f>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>IF(H2&gt;85000, "High","Low")</f>
+        <v>High</v>
+      </c>
+      <c r="R2" t="str" cm="1">
+        <f t="array" ref="R2">_xlfn.IFS($H2="", "No Data", $H2&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="46">
         <v>45097.915243055562</v>
       </c>
       <c r="C3" s="27" t="s">
@@ -2895,12 +2956,44 @@
       <c r="J3" s="27" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:L21" si="0">IF($A3=K$1, "Role Desired", "Not Desired")</f>
+        <v>Role Desired</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M21" si="1">IF($A3=K$1, "Role Desired", IF($A3=L$1, "Role Desired", "Not Desired"))</f>
+        <v>Role Desired</v>
+      </c>
+      <c r="N3" t="b">
+        <f t="shared" ref="N3:N21" si="2">AND($A3=$K$1,$A3=$L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <f t="shared" ref="O3:O21" si="3">OR($A3=$K$1, $A3=$L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P21" si="4">IF(OR($A3=$K$1, $A3=$L$1), "Role Desired", "Not Desired")</f>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q21" si="5">IF(H3&gt;85000, "High","Low")</f>
+        <v>Low</v>
+      </c>
+      <c r="R3" t="str" cm="1">
+        <f t="array" ref="R3">_xlfn.IFS($H3="", "No Data", $H3&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary Low</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="46">
         <v>45173.250416666669</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -2925,12 +3018,44 @@
       <c r="J4" s="27" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R4" t="str" cm="1">
+        <f t="array" ref="R4">_xlfn.IFS($H4="", "No Data", $H4&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="46">
         <v>45156.253321759257</v>
       </c>
       <c r="C5" s="27" t="s">
@@ -2955,12 +3080,44 @@
       <c r="J5" s="27" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N5" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q5" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R5" t="str" cm="1">
+        <f t="array" ref="R5">_xlfn.IFS($H5="", "No Data", $H5&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="46">
         <v>45147.802951388891</v>
       </c>
       <c r="C6" s="27" t="s">
@@ -2985,12 +3142,44 @@
       <c r="J6" s="27" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N6" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R6" t="str" cm="1">
+        <f t="array" ref="R6">_xlfn.IFS($H6="", "No Data", $H6&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="46">
         <v>45202.753101851849</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -3015,12 +3204,44 @@
       <c r="J7" s="27" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N7" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q7" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R7" t="str" cm="1">
+        <f t="array" ref="R7">_xlfn.IFS($H7="", "No Data", $H7&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="46">
         <v>44949.850462962961</v>
       </c>
       <c r="C8" s="27" t="s">
@@ -3045,12 +3266,44 @@
       <c r="J8" s="27" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N8" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O8" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q8" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R8" t="str" cm="1">
+        <f t="array" ref="R8">_xlfn.IFS($H8="", "No Data", $H8&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="46">
         <v>45001.627175925933</v>
       </c>
       <c r="C9" s="27" t="s">
@@ -3077,12 +3330,44 @@
       <c r="J9" s="27" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N9" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O9" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q9" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R9" t="str" cm="1">
+        <f t="array" ref="R9">_xlfn.IFS($H9="", "No Data", $H9&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="46">
         <v>45041.375868055547</v>
       </c>
       <c r="C10" s="27" t="s">
@@ -3107,12 +3392,44 @@
       <c r="J10" s="27" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N10" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O10" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q10" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R10" t="str" cm="1">
+        <f t="array" ref="R10">_xlfn.IFS($H10="", "No Data", $H10&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="46">
         <v>45106.587094907409</v>
       </c>
       <c r="C11" s="27" t="s">
@@ -3139,12 +3456,44 @@
       <c r="J11" s="27" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N11" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O11" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q11" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R11" t="str" cm="1">
+        <f t="array" ref="R11">_xlfn.IFS($H11="", "No Data", $H11&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="46">
         <v>45029.919687499998</v>
       </c>
       <c r="C12" s="27" t="s">
@@ -3171,12 +3520,44 @@
       <c r="J12" s="27" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N12" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O12" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q12" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R12" t="str" cm="1">
+        <f t="array" ref="R12">_xlfn.IFS($H12="", "No Data", $H12&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="46">
         <v>45091.502789351849</v>
       </c>
       <c r="C13" s="27" t="s">
@@ -3203,12 +3584,44 @@
       <c r="J13" s="27" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N13" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O13" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q13" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R13" t="str" cm="1">
+        <f t="array" ref="R13">_xlfn.IFS($H13="", "No Data", $H13&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="46">
         <v>45175.543124999997</v>
       </c>
       <c r="C14" s="27" t="s">
@@ -3235,12 +3648,44 @@
       <c r="J14" s="27" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N14" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O14" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q14" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R14" t="str" cm="1">
+        <f t="array" ref="R14">_xlfn.IFS($H14="", "No Data", $H14&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="46">
         <v>45117.778391203698</v>
       </c>
       <c r="C15" s="27" t="s">
@@ -3267,12 +3712,44 @@
       <c r="J15" s="27" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N15" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O15" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q15" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R15" t="str" cm="1">
+        <f t="array" ref="R15">_xlfn.IFS($H15="", "No Data", $H15&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary Low</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="46">
         <v>44938.614351851851</v>
       </c>
       <c r="C16" s="27" t="s">
@@ -3299,12 +3776,44 @@
       <c r="J16" s="27" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N16" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O16" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q16" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R16" t="str" cm="1">
+        <f t="array" ref="R16">_xlfn.IFS($H16="", "No Data", $H16&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="46">
         <v>44985.354097222233</v>
       </c>
       <c r="C17" s="27" t="s">
@@ -3331,12 +3840,44 @@
       <c r="J17" s="27" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N17" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O17" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q17" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R17" t="str" cm="1">
+        <f t="array" ref="R17">_xlfn.IFS($H17="", "No Data", $H17&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B18" s="46">
         <v>45063.792291666658</v>
       </c>
       <c r="C18" s="27" t="s">
@@ -3361,12 +3902,44 @@
       <c r="J18" s="27" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N18" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O18" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q18" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R18" t="str" cm="1">
+        <f t="array" ref="R18">_xlfn.IFS($H18="", "No Data", $H18&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="46">
         <v>45017.004837962973</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -3393,12 +3966,44 @@
       <c r="J19" s="27" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N19" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O19" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q19" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R19" t="str" cm="1">
+        <f t="array" ref="R19">_xlfn.IFS($H19="", "No Data", $H19&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="46">
         <v>45169.64203703704</v>
       </c>
       <c r="C20" s="27" t="s">
@@ -3423,12 +4028,44 @@
       <c r="J20" s="27" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="1"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="N20" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O20" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="4"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="Q20" t="str">
+        <f t="shared" si="5"/>
+        <v>Low</v>
+      </c>
+      <c r="R20" t="str" cm="1">
+        <f t="array" ref="R20">_xlfn.IFS($H20="", "No Data", $H20&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>No Data</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="47">
+      <c r="B21" s="46">
         <v>45000.542685185188</v>
       </c>
       <c r="C21" s="27" t="s">
@@ -3455,9 +4092,42 @@
       <c r="J21" s="27" t="s">
         <v>135</v>
       </c>
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>Not Desired</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="0"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="1"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="N21" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O21" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="4"/>
+        <v>Role Desired</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" si="5"/>
+        <v>High</v>
+      </c>
+      <c r="R21" t="str" cm="1">
+        <f t="array" ref="R21">_xlfn.IFS($H21="", "No Data", $H21&gt;=$Q$1,"salary &gt; 85k", TRUE,"salary Low")</f>
+        <v>salary &gt; 85k</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3467,29 +4137,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.41796875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="21.83984375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.15625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="38.15625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.578125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="18.578125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="68.15625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="68.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>46</v>
       </c>
@@ -3514,7 +4184,7 @@
       <c r="H1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="45" t="s">
         <v>54</v>
       </c>
       <c r="J1" s="34" t="s">
@@ -3549,11 +4219,11 @@
         <v>85000</v>
       </c>
     </row>
-    <row r="2" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="46">
         <v>44996.547291666669</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -3613,11 +4283,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="3" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="46">
         <v>45097.915243055562</v>
       </c>
       <c r="C3" s="27" t="s">
@@ -3677,11 +4347,11 @@
         <v>Salary Low</v>
       </c>
     </row>
-    <row r="4" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="46">
         <v>45173.250416666669</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -3739,11 +4409,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="5" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="46">
         <v>45156.253321759257</v>
       </c>
       <c r="C5" s="27" t="s">
@@ -3801,11 +4471,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="6" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="46">
         <v>45147.802951388891</v>
       </c>
       <c r="C6" s="27" t="s">
@@ -3863,11 +4533,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="7" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="47">
+      <c r="B7" s="46">
         <v>45202.753101851849</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -3925,11 +4595,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="8" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="46">
         <v>44949.850462962961</v>
       </c>
       <c r="C8" s="27" t="s">
@@ -3987,11 +4657,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="9" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="47">
+      <c r="B9" s="46">
         <v>45001.627175925933</v>
       </c>
       <c r="C9" s="27" t="s">
@@ -4051,11 +4721,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="10" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="47">
+      <c r="B10" s="46">
         <v>45041.375868055547</v>
       </c>
       <c r="C10" s="27" t="s">
@@ -4113,11 +4783,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="11" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="47">
+      <c r="B11" s="46">
         <v>45106.587094907409</v>
       </c>
       <c r="C11" s="27" t="s">
@@ -4177,11 +4847,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="12" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="47">
+      <c r="B12" s="46">
         <v>45029.919687499998</v>
       </c>
       <c r="C12" s="27" t="s">
@@ -4241,11 +4911,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="13" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="46">
         <v>45091.502789351849</v>
       </c>
       <c r="C13" s="27" t="s">
@@ -4305,11 +4975,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="14" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="46">
         <v>45175.543124999997</v>
       </c>
       <c r="C14" s="27" t="s">
@@ -4369,11 +5039,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="15" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="47">
+      <c r="B15" s="46">
         <v>45117.778391203698</v>
       </c>
       <c r="C15" s="27" t="s">
@@ -4433,11 +5103,11 @@
         <v>Salary Low</v>
       </c>
     </row>
-    <row r="16" spans="1:18 16384:16384" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18 16384:16384" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="47">
+      <c r="B16" s="46">
         <v>44938.614351851851</v>
       </c>
       <c r="C16" s="27" t="s">
@@ -4497,11 +5167,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47">
+      <c r="B17" s="46">
         <v>44985.354097222233</v>
       </c>
       <c r="C17" s="27" t="s">
@@ -4561,11 +5231,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="47">
+      <c r="B18" s="46">
         <v>45063.792291666658</v>
       </c>
       <c r="C18" s="27" t="s">
@@ -4623,11 +5293,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="47">
+      <c r="B19" s="46">
         <v>45017.004837962973</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -4687,11 +5357,11 @@
         <v>Salary &gt; 85K</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="47">
+      <c r="B20" s="46">
         <v>45169.64203703704</v>
       </c>
       <c r="C20" s="27" t="s">
@@ -4749,11 +5419,11 @@
         <v>No Data</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="47">
+      <c r="B21" s="46">
         <v>45000.542685185188</v>
       </c>
       <c r="C21" s="27" t="s">
@@ -4827,17 +5497,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.578125" customWidth="1"/>
-    <col min="2" max="2" width="13.41796875" customWidth="1"/>
-    <col min="3" max="3" width="31.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="26" t="s">
         <v>28</v>
       </c>
@@ -4847,14 +5517,14 @@
       <c r="D2" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="43" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="27" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
@@ -4874,7 +5544,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="e">
         <f>A4 + "text"</f>
         <v>#VALUE!</v>
@@ -4894,7 +5564,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -4914,7 +5584,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="e" cm="1">
         <f t="array" aca="1" ref="B6" ca="1">COUNTT(A3:A9)</f>
         <v>#NAME?</v>
@@ -4934,7 +5604,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="27" t="e">
         <f>VLOOKUP("Value", A1:A10, 2, FALSE)</f>
         <v>#N/A</v>
@@ -4954,7 +5624,7 @@
         <v>This hides #N/A error</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="27" t="e">
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
@@ -4974,7 +5644,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="27" t="e">
         <f>SUM(A1:A10 C1:C10)</f>
         <v>#NULL!</v>
@@ -5003,32 +5673,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B83CC08-3BAC-45FD-A105-07186D54808A}">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="D2:E2"/>
+    <sheetView showGridLines="0" zoomScale="242" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.578125" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="36" t="s">
         <v>137</v>
       </c>
       <c r="C2" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="44" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="38" t="b">
         <v>1</v>
       </c>
@@ -5044,7 +5714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="38" t="b">
         <v>1</v>
       </c>
@@ -5060,7 +5730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="38" t="b">
         <v>0</v>
       </c>
@@ -5076,23 +5746,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="b">
         <v>0</v>
       </c>
       <c r="C6" s="41" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="43" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="43" t="b">
+      <c r="D6" s="42" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="42" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>